<commit_message>
Aufgabenliste fuer 2.Woche upgedated
</commit_message>
<xml_diff>
--- a/Aufgabenliste1.xlsx
+++ b/Aufgabenliste1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Google Drive\Schule\4BHWII\SWP1\WebProject\respo\Project4BHWII_Webproject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\GitRepos\Project4BHWII_Webproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEB9E73-B3D9-41D5-82E5-B976D939C951}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FF1809-262C-4513-8AA5-20FC63E8F72E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{F23AB310-9AEA-4EDF-A171-415F0C0F6266}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F23AB310-9AEA-4EDF-A171-415F0C0F6266}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Thema:</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Recherge/Implementieren des adaptiven Headers</t>
+  </si>
+  <si>
+    <t>Navbar implementiren + Design erweitern</t>
   </si>
 </sst>
 </file>
@@ -445,12 +451,13 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="7" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="54.77734375" customWidth="1"/>
+    <col min="3" max="7" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -458,7 +465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -469,19 +476,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -501,7 +508,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -521,23 +528,38 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4">
+        <v>43852</v>
+      </c>
+      <c r="F10" s="4">
+        <v>43858</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="4">
+        <v>43852</v>
+      </c>
+      <c r="F11" s="4">
+        <v>43858</v>
+      </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -545,7 +567,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -553,7 +575,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -561,7 +583,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -569,7 +591,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -577,7 +599,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -585,7 +607,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -593,7 +615,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -601,7 +623,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -609,7 +631,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -617,7 +639,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -625,7 +647,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -633,7 +655,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -641,7 +663,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>

</xml_diff>

<commit_message>
Footer hinzugefügt, Backgroundcolor hinz
</commit_message>
<xml_diff>
--- a/Aufgabenliste1.xlsx
+++ b/Aufgabenliste1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\GitRepos\Project4BHWII_Webproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FF1809-262C-4513-8AA5-20FC63E8F72E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC2C3D1-2C8D-4773-90C9-0807C28A7526}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F23AB310-9AEA-4EDF-A171-415F0C0F6266}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>Thema:</t>
   </si>
@@ -448,7 +448,7 @@
   <dimension ref="B2:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,7 +541,9 @@
       <c r="F10" s="4">
         <v>43858</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
@@ -557,7 +559,9 @@
       <c r="F11" s="4">
         <v>43858</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>

</xml_diff>